<commit_message>
Small change in SVM Excel file
</commit_message>
<xml_diff>
--- a/LaTex/data/svm_radial_k.xlsx
+++ b/LaTex/data/svm_radial_k.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="12">
   <si>
     <t>edicted</t>
   </si>
@@ -388,15 +388,12 @@
   <dimension ref="B2:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:X14"/>
+      <selection activeCell="C13" sqref="C13:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
       <c r="C2">
         <v>0</v>
       </c>

</xml_diff>